<commit_message>
logic test and full J17  test
</commit_message>
<xml_diff>
--- a/tests/DB/MTC_AFT/J17_Armant_1.xlsx
+++ b/tests/DB/MTC_AFT/J17_Armant_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ArduinoProject\IO_Tester\tests\DB\MTC_AFT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70670125-1680-4219-9996-E3AF6C2E6734}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87AF0B92-80BC-4109-B9BE-F9A73B5AF89E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="29">
   <si>
     <t>Row</t>
   </si>
@@ -79,18 +79,12 @@
     <t>Circuit Diagram Reference</t>
   </si>
   <si>
-    <t>logic input</t>
-  </si>
-  <si>
     <t>Power_Expected</t>
   </si>
   <si>
     <t>PullUp_Expected</t>
   </si>
   <si>
-    <t>"none"</t>
-  </si>
-  <si>
     <t>Test_Result</t>
   </si>
   <si>
@@ -100,10 +94,34 @@
     <t>Power_Input</t>
   </si>
   <si>
-    <t>C1_AO5V10</t>
-  </si>
-  <si>
-    <t>C1_AO2V10</t>
+    <t>PullUp_Input</t>
+  </si>
+  <si>
+    <t>C2_DO13_1</t>
+  </si>
+  <si>
+    <t>C2_DO14_1</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>C1_AO5_10</t>
+  </si>
+  <si>
+    <t>C1_AO2_10</t>
+  </si>
+  <si>
+    <t>logic_input</t>
+  </si>
+  <si>
+    <t>Logic_Expected</t>
+  </si>
+  <si>
+    <t>C4_DI29_0</t>
+  </si>
+  <si>
+    <t>C4_DI30_0</t>
   </si>
 </sst>
 </file>
@@ -134,7 +152,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -144,6 +162,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -334,7 +358,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -385,6 +409,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -691,10 +718,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L51"/>
+  <dimension ref="A1:N51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -707,13 +734,14 @@
     <col min="6" max="6" width="20.85546875" style="1" customWidth="1"/>
     <col min="7" max="7" width="24.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="17.7109375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="22.140625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="14" style="1" customWidth="1"/>
-    <col min="12" max="12" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="9" style="1"/>
+    <col min="10" max="11" width="22.140625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="14" style="1" customWidth="1"/>
+    <col min="13" max="13" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
@@ -736,22 +764,28 @@
         <v>13</v>
       </c>
       <c r="H1" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="I1" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="J1" s="10" t="s">
+      <c r="K1" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="N1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="K1" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="9">
         <v>1</v>
       </c>
@@ -777,17 +811,17 @@
         <v>24</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="J2" s="10"/>
-      <c r="K2" s="3" t="s">
+      <c r="K2" s="10"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="L2" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="9">
         <v>2</v>
       </c>
@@ -812,18 +846,20 @@
       <c r="H3" s="14">
         <v>0</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="I3" s="3"/>
+      <c r="J3" s="10">
+        <v>20</v>
+      </c>
+      <c r="K3" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="J3" s="10"/>
-      <c r="K3" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="9">
         <v>3</v>
       </c>
@@ -848,18 +884,20 @@
       <c r="H4" s="14">
         <v>0</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="I4" s="3"/>
+      <c r="J4" s="10">
+        <v>20</v>
+      </c>
+      <c r="K4" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="J4" s="10"/>
-      <c r="K4" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="9">
         <v>4</v>
       </c>
@@ -884,18 +922,20 @@
       <c r="H5" s="14">
         <v>0</v>
       </c>
-      <c r="I5" s="3" t="s">
+      <c r="I5" s="3"/>
+      <c r="J5" s="10">
+        <v>20</v>
+      </c>
+      <c r="K5" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="J5" s="10"/>
-      <c r="K5" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="L5" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="9">
         <v>5</v>
       </c>
@@ -921,17 +961,17 @@
         <v>5</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="J6" s="10"/>
-      <c r="K6" s="3" t="s">
+      <c r="K6" s="10"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="L6" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="9">
         <v>6</v>
       </c>
@@ -953,21 +993,23 @@
       <c r="G7" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="14">
+      <c r="H7" s="18">
         <v>0</v>
       </c>
-      <c r="I7" s="3" t="s">
+      <c r="I7" s="3"/>
+      <c r="J7" s="10">
+        <v>0</v>
+      </c>
+      <c r="K7" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="J7" s="10"/>
-      <c r="K7" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="L7" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="9">
         <v>7</v>
       </c>
@@ -992,18 +1034,20 @@
       <c r="H8" s="14">
         <v>0</v>
       </c>
-      <c r="I8" s="3" t="s">
+      <c r="I8" s="3"/>
+      <c r="J8" s="10">
+        <v>0</v>
+      </c>
+      <c r="K8" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="L8" s="3"/>
+      <c r="M8" s="3"/>
+      <c r="N8" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="J8" s="10"/>
-      <c r="K8" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="L8" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="9">
         <v>8</v>
       </c>
@@ -1028,18 +1072,20 @@
       <c r="H9" s="14">
         <v>3.5</v>
       </c>
-      <c r="I9" s="3" t="s">
+      <c r="I9" s="3"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="10"/>
+      <c r="L9" s="3">
+        <v>3</v>
+      </c>
+      <c r="M9" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="N9" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="J9" s="10"/>
-      <c r="K9" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="L9" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="9">
         <v>9</v>
       </c>
@@ -1064,18 +1110,20 @@
       <c r="H10" s="14">
         <v>3.5</v>
       </c>
-      <c r="I10" s="3" t="s">
+      <c r="I10" s="3"/>
+      <c r="J10" s="10"/>
+      <c r="K10" s="10"/>
+      <c r="L10" s="3">
+        <v>3</v>
+      </c>
+      <c r="M10" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="N10" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="J10" s="10"/>
-      <c r="K10" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="L10" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="11">
         <v>10</v>
       </c>
@@ -1086,7 +1134,7 @@
       <c r="F11" s="12"/>
       <c r="G11" s="13"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -1097,7 +1145,7 @@
       <c r="F12" s="3"/>
       <c r="G12" s="4"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -1108,7 +1156,7 @@
       <c r="F13" s="3"/>
       <c r="G13" s="4"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -1119,7 +1167,7 @@
       <c r="F14" s="3"/>
       <c r="G14" s="4"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -1130,7 +1178,7 @@
       <c r="F15" s="3"/>
       <c r="G15" s="4"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>15</v>
       </c>

</xml_diff>